<commit_message>
s3 implementation, finishing auth, forms creations, file managment
</commit_message>
<xml_diff>
--- a/dbstructure.xlsx
+++ b/dbstructure.xlsx
@@ -8,23 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bahai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434C0809-43D0-424E-A5F2-8B3B5D64D6C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682151C3-A630-4E06-99E2-B26347EDF052}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="11" xr2:uid="{8323B724-EE66-4869-A2CF-045A26A2E818}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="9" activeTab="12" xr2:uid="{8323B724-EE66-4869-A2CF-045A26A2E818}"/>
   </bookViews>
   <sheets>
     <sheet name="initials notes" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
     <sheet name="configurations" sheetId="9" r:id="rId3"/>
-    <sheet name="groups" sheetId="3" r:id="rId4"/>
-    <sheet name="groups_participants" sheetId="4" r:id="rId5"/>
-    <sheet name="messages" sheetId="7" r:id="rId6"/>
-    <sheet name="books" sheetId="5" r:id="rId7"/>
-    <sheet name="book_images" sheetId="11" r:id="rId8"/>
-    <sheet name="available_times" sheetId="6" r:id="rId9"/>
-    <sheet name="logs_stepped_down_hosts" sheetId="12" r:id="rId10"/>
-    <sheet name="logs_connections" sheetId="10" r:id="rId11"/>
+    <sheet name="groups_participants" sheetId="4" r:id="rId4"/>
+    <sheet name="messages" sheetId="7" r:id="rId5"/>
+    <sheet name="books" sheetId="5" r:id="rId6"/>
+    <sheet name="book_images" sheetId="11" r:id="rId7"/>
+    <sheet name="available_times" sheetId="6" r:id="rId8"/>
+    <sheet name="logs_stepped_down_hosts" sheetId="12" r:id="rId9"/>
+    <sheet name="logs_connections" sheetId="10" r:id="rId10"/>
+    <sheet name="groups" sheetId="3" r:id="rId11"/>
     <sheet name="logs_configurations" sheetId="13" r:id="rId12"/>
+    <sheet name="group_containers" sheetId="14" r:id="rId13"/>
+    <sheet name="autors_containers" sheetId="16" r:id="rId14"/>
+    <sheet name="autors" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +53,25 @@
     <author>tc={3B19B1CC-7029-490D-8955-069A8E9531DA}</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{3B19B1CC-7029-490D-8955-069A8E9531DA}">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{3B19B1CC-7029-490D-8955-069A8E9531DA}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    define length</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0556A122-B696-48C1-876E-31CE9778CA87}</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{0556A122-B696-48C1-876E-31CE9778CA87}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="144">
   <si>
     <t>tables</t>
   </si>
@@ -451,7 +472,53 @@
     <t>0 - dropped</t>
   </si>
   <si>
-    <t>USER_ID</t>
+    <t>autor_id</t>
+  </si>
+  <si>
+    <t>group_container_id</t>
+  </si>
+  <si>
+    <t>group_containers</t>
+  </si>
+  <si>
+    <t>autors_in_containers</t>
+  </si>
+  <si>
+    <t>autors</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>container name</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>containers will have a weight, and all containers will appear on the homepage ordered by weight</t>
+  </si>
+  <si>
+    <t>user that created the container</t>
+  </si>
+  <si>
+    <t>descritpion</t>
+  </si>
+  <si>
+    <t>optional description for the container</t>
+  </si>
+  <si>
+    <t>id of autor to link into container</t>
+  </si>
+  <si>
+    <t>id of container that link with autor</t>
+  </si>
+  <si>
+    <t>1. is active
+0. was deleted</t>
   </si>
 </sst>
 </file>
@@ -494,7 +561,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -648,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -688,6 +755,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -709,15 +786,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,7 +804,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,7 +1142,15 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D3" dT="2021-02-03T11:44:51.95" personId="{AAC854CB-10E5-43F5-9EA2-A51A9B46D685}" id="{3B19B1CC-7029-490D-8955-069A8E9531DA}">
+  <threadedComment ref="E3" dT="2021-02-03T11:44:51.95" personId="{AAC854CB-10E5-43F5-9EA2-A51A9B46D685}" id="{3B19B1CC-7029-490D-8955-069A8E9531DA}">
+    <text>define length</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E3" dT="2021-02-03T11:44:51.95" personId="{AAC854CB-10E5-43F5-9EA2-A51A9B46D685}" id="{0556A122-B696-48C1-876E-31CE9778CA87}">
     <text>define length</text>
   </threadedComment>
 </ThreadedComments>
@@ -1153,128 +1246,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161F0660-1BD8-420C-B975-B2C0C0425302}">
-  <dimension ref="A1:F22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="4" width="30.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D8" s="2"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D22" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:F2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2821E0-22F5-43AD-A369-A35CF4C2EA5B}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1288,20 +1259,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
@@ -1358,13 +1329,13 @@
       <c r="A6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="21" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1386,12 +1357,191 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94045C2E-C635-4A18-A334-E819565FDA66}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="9" width="30.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382E7894-7A55-47AE-8396-9F54CED91927}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,6 +1550,388 @@
       <c r="A1" s="2"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A2EBA0-7AA6-4639-B2C8-37BD373C71C2}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F58B472-D234-469D-A88E-F07C282F4A44}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFB6458-0991-49D3-9396-1B727F6D3067}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1408,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E11F77-5098-457C-83ED-544D3BCF07EB}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="A1:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1421,19 +1953,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="14"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -1626,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A418C6-F26A-4B77-9CD8-A6F548F8028B}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1636,18 +2168,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -1793,170 +2325,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94045C2E-C635-4A18-A334-E819565FDA66}">
-  <dimension ref="A1:J12"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="8" width="30.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:J1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4DD0B1-B748-40B7-89AF-0972D98AF87A}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1971,24 +2339,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
@@ -2105,7 +2473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D238392A-1613-4D10-9CB9-169151E566DB}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -2120,25 +2488,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -2228,45 +2596,47 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B92BB0-70C2-496A-BABE-36FE24978C15}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="6" width="30.77734375" customWidth="1"/>
+    <col min="1" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="7" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="31"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
       <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="34"/>
+      <c r="I1" s="34"/>
+    </row>
+    <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="37"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>19</v>
       </c>
@@ -2274,97 +2644,103 @@
         <v>128</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
         <v>87</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" s="9" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="11"/>
       <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:H2"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E869E6D-A5B1-4539-9DB3-AF4512991B54}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2380,22 +2756,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
@@ -2464,7 +2840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47046AFD-33B9-4884-B24B-1AE28F753E50}">
   <dimension ref="A1:M8"/>
   <sheetViews>
@@ -2479,26 +2855,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:13" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -2616,10 +2992,10 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="28"/>
+      <c r="M7" s="38"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
@@ -2643,8 +3019,8 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2654,4 +3030,126 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161F0660-1BD8-420C-B975-B2C0C0425302}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="4" width="30.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>